<commit_message>
more adjustments to ACH
</commit_message>
<xml_diff>
--- a/data/raw/ACH/ACH_Payment.xlsx
+++ b/data/raw/ACH/ACH_Payment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\ACH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\ACH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D526F617-922F-4C58-A3BA-6B7AE5C46F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DF89B0-54D1-466A-9EF3-0BAAE3DF7438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12830" yWindow="4120" windowWidth="29780" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="823" windowWidth="18514" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Wood, Steve</t>
-  </si>
-  <si>
     <t>Invoice Number</t>
   </si>
   <si>
@@ -59,64 +56,16 @@
     <t>Clean Harbors</t>
   </si>
   <si>
-    <t>Czysz 2</t>
-  </si>
-  <si>
-    <t>6/1/2024</t>
-  </si>
-  <si>
-    <t>Rent</t>
-  </si>
-  <si>
-    <t>Interest Payment</t>
-  </si>
-  <si>
-    <t>3460 Rockefeller Ct.</t>
-  </si>
-  <si>
-    <t>1004976013</t>
-  </si>
-  <si>
-    <t>Crystal Clean</t>
-  </si>
-  <si>
-    <t>18610831</t>
-  </si>
-  <si>
-    <t>18658565</t>
-  </si>
-  <si>
-    <t>Spheeris</t>
-  </si>
-  <si>
-    <t>5/31/2024</t>
-  </si>
-  <si>
-    <t>BARSTOW 5/6 - 5/9</t>
-  </si>
-  <si>
-    <t>McCrea</t>
-  </si>
-  <si>
-    <t>5/31/2024 - 1</t>
-  </si>
-  <si>
-    <t>HONOLULU 5/14 - 5/17</t>
-  </si>
-  <si>
-    <t>5/31/2024 - 2</t>
-  </si>
-  <si>
-    <t>CHINHEA 5/20-5/24</t>
-  </si>
-  <si>
-    <t>WHIDBEY 5/20-5/24</t>
-  </si>
-  <si>
-    <t>Sonnier, Eddie</t>
-  </si>
-  <si>
-    <t>EL CENTRO 5/20-5/23</t>
+    <t>Republic</t>
+  </si>
+  <si>
+    <t>New Pig</t>
+  </si>
+  <si>
+    <t>1004985554</t>
+  </si>
+  <si>
+    <t>24256823-00</t>
   </si>
 </sst>
 </file>
@@ -124,9 +73,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +104,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -190,7 +146,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -476,228 +435,138 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1007551</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45324</v>
+      </c>
+      <c r="D2" s="5">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45352</v>
+      </c>
+      <c r="D3" s="5">
+        <v>15139.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7">
-        <v>45444</v>
-      </c>
-      <c r="D2" s="5">
-        <v>17500</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7">
-        <v>45343</v>
-      </c>
-      <c r="D3" s="6">
-        <v>13881.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="7">
-        <v>45387</v>
-      </c>
-      <c r="D4" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="7">
-        <v>45415</v>
-      </c>
-      <c r="D5" s="6">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7">
-        <v>45421</v>
-      </c>
-      <c r="D6" s="5">
-        <v>352</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="7">
-        <v>45429</v>
-      </c>
-      <c r="D7" s="5">
-        <v>883.88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7">
-        <v>45436</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1518.88</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7">
-        <v>45436</v>
-      </c>
-      <c r="D9" s="5">
-        <v>383.5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="7">
-        <v>45436</v>
-      </c>
-      <c r="D10" s="5">
-        <v>383.5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="7">
-        <v>45435</v>
-      </c>
-      <c r="D11" s="5">
-        <v>517.41999999999996</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7">
-        <v>45444</v>
-      </c>
-      <c r="D12" s="5">
-        <v>11000</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45245</v>
+      </c>
+      <c r="D4" s="5">
+        <v>11338.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" s="3"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
     </row>
   </sheetData>

</xml_diff>